<commit_message>
Minor adjustments + Bug fixes
</commit_message>
<xml_diff>
--- a/runs/hyperparameters.xlsx
+++ b/runs/hyperparameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diogo\Desktop\DenseNet-PyTorch\runs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ImageLab\Desktop\DenseNet-PyTorch\runs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F1C3E1-52E5-4700-A107-B5577F19779E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38429662-C8F0-45E8-B145-F1B4D9243609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8880" xr2:uid="{B2BB1A88-F285-4939-A9F6-909F0CBA447B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{B2BB1A88-F285-4939-A9F6-909F0CBA447B}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -100,6 +100,21 @@
   </si>
   <si>
     <t>python main.py --layers 100 --growth 12 --reduce 0.5 --test DenseNet-BC-100-12</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>CIFAR-10</t>
+  </si>
+  <si>
+    <t>ImageNet</t>
+  </si>
+  <si>
+    <t>DenseNet-121</t>
+  </si>
+  <si>
+    <t>python main.py --layers 121 --growth 32 --reduce 0.5 --epochs 90 -b 256 --name DenseNet-121 --imagenet</t>
   </si>
 </sst>
 </file>
@@ -476,27 +491,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D59319DB-CBDE-4CFE-8FA0-53DD6872609D}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" style="2" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" customWidth="1"/>
-    <col min="5" max="5" width="6.88671875" customWidth="1"/>
-    <col min="6" max="6" width="8.109375" customWidth="1"/>
-    <col min="7" max="7" width="6.44140625" customWidth="1"/>
-    <col min="8" max="9" width="7.5546875" customWidth="1"/>
-    <col min="10" max="10" width="8.109375" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" style="7"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" customWidth="1"/>
+    <col min="8" max="9" width="7.5703125" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -533,11 +548,14 @@
       <c r="L1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -574,11 +592,14 @@
       <c r="L2" s="1">
         <v>64</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
@@ -615,11 +636,14 @@
       <c r="L3" s="1">
         <v>64</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -656,37 +680,80 @@
       <c r="L4" s="1">
         <v>64</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="M4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="M5" s="7"/>
-    </row>
-    <row r="6" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="M6" s="7"/>
-    </row>
-    <row r="7" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N5" s="7"/>
+    </row>
+    <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="E6" s="1">
+        <v>121</v>
+      </c>
+      <c r="F6" s="1">
+        <v>32</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="1">
+        <v>90</v>
+      </c>
+      <c r="L6" s="1">
+        <v>256</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="M7" s="7"/>
-    </row>
-    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N7" s="7"/>
+    </row>
+    <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="M8" s="7"/>
-    </row>
-    <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="M9" s="7"/>
-    </row>
-    <row r="10" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N9" s="7"/>
+    </row>
+    <row r="10" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="M10" s="7"/>
-    </row>
-    <row r="11" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N10" s="7"/>
+    </row>
+    <row r="11" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>